<commit_message>
Added signs of non-production unit and "personal data".
</commit_message>
<xml_diff>
--- a/Parameters/ProjectsSubTypesDescriptions.xlsx
+++ b/Parameters/ProjectsSubTypesDescriptions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1521E9-C115-4198-A6AB-3B074E0AB068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E20D8-8F42-4583-B805-A7B1D905783C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>От</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Командировки (рабочее время в пути)</t>
+  </si>
+  <si>
+    <t>ProjectSubTypePersData</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyProtection="1">
@@ -196,6 +199,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -480,209 +495,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F53492B-E9B6-44FD-A10D-37455B40CAC6}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>